<commit_message>
adding testing versions of spreadsheets
</commit_message>
<xml_diff>
--- a/feedback_forms/testing_versions/landfill_operator_feedback_v070_with_errors_02.xlsx
+++ b/feedback_forms/testing_versions/landfill_operator_feedback_v070_with_errors_02.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/tony_held_arb_ca_gov/Documents/code/pycharm/feedback_portal/feedback_forms/testing_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{0BB98C50-23F5-43F3-BCBC-FF70E147074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{745A5253-7539-4DA7-9B0D-F36E647013AC}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{0BB98C50-23F5-43F3-BCBC-FF70E147074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E25838A7-6316-4776-AD77-B8CD8ECA7FC5}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="vY3M817KAomZyhlm4oS6cOyuUSxWaTaz7lVX62BALQGX5cCDz411RVbfnvbnpvf21HlxJBaGYtmscNkzHgnKag==" workbookSaltValue="+DW2WdW8uRq+VBPkAiodVA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="2687" yWindow="460" windowWidth="19200" windowHeight="11093" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="4547" yWindow="2500" windowWidth="19200" windowHeight="11093" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -3494,10 +3494,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88E4CF48-AAEC-4756-B8D6-56F7F8A93943}" name="_issue_tracking_Table_01" displayName="_issue_tracking_Table_01" ref="B9:C13" totalsRowShown="0">
   <autoFilter ref="B9:C13" xr:uid="{24D72A52-95E4-464B-93BB-49FD17A99B8E}"/>
@@ -4269,7 +4265,7 @@
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="56">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E32" s="50"/>
       <c r="G32" s="36"/>
@@ -10002,6 +9998,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -10236,7 +10243,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -10245,18 +10252,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC83B422-5B73-4269-9006-1DDE9C149499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10275,21 +10282,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
making the importing process more resilient to bad data and types
</commit_message>
<xml_diff>
--- a/feedback_forms/testing_versions/landfill_operator_feedback_v070_with_errors_02.xlsx
+++ b/feedback_forms/testing_versions/landfill_operator_feedback_v070_with_errors_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/tony_held_arb_ca_gov/Documents/code/pycharm/feedback_portal/feedback_forms/testing_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{0BB98C50-23F5-43F3-BCBC-FF70E147074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E25838A7-6316-4776-AD77-B8CD8ECA7FC5}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{0BB98C50-23F5-43F3-BCBC-FF70E147074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA690751-B54B-4DA8-9261-F1EFC560B0E3}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="vY3M817KAomZyhlm4oS6cOyuUSxWaTaz7lVX62BALQGX5cCDz411RVbfnvbnpvf21HlxJBaGYtmscNkzHgnKag==" workbookSaltValue="+DW2WdW8uRq+VBPkAiodVA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="4547" yWindow="2500" windowWidth="19200" windowHeight="11093" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="442">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2034,46 +2034,46 @@
     </r>
   </si>
   <si>
-    <t>{{ emission_cause }}</t>
-  </si>
-  <si>
-    <t>{{ emission_cause_secondary }}</t>
-  </si>
-  <si>
-    <t>{{ emission_cause_tertiary }}</t>
-  </si>
-  <si>
-    <t>{{ emission_identified_flag_fk }}</t>
-  </si>
-  <si>
-    <t>{{ emission_location }}</t>
-  </si>
-  <si>
-    <t>{{ emission_type_fk }}</t>
-  </si>
-  <si>
-    <t>{{ id_incidence }}</t>
-  </si>
-  <si>
-    <t>{{ id_message }}</t>
-  </si>
-  <si>
-    <t>{{ id_plume }}</t>
-  </si>
-  <si>
-    <t>{{ included_in_last_lmr }}</t>
-  </si>
-  <si>
-    <t>{{ lat_carb }}</t>
-  </si>
-  <si>
-    <t>{{ long_carb }}</t>
-  </si>
-  <si>
-    <t>{{ observation_timestamp }}</t>
-  </si>
-  <si>
-    <t>{{ planned_for_next_lmr }}</t>
+    <t>string 2</t>
+  </si>
+  <si>
+    <t>string 3</t>
+  </si>
+  <si>
+    <t>string 4</t>
+  </si>
+  <si>
+    <t>string 5</t>
+  </si>
+  <si>
+    <t>string q4</t>
+  </si>
+  <si>
+    <t>string 10</t>
+  </si>
+  <si>
+    <t>string 11</t>
+  </si>
+  <si>
+    <t>string 12</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>1563.987</t>
+  </si>
+  <si>
+    <t>q28</t>
+  </si>
+  <si>
+    <t>02/33/2025</t>
+  </si>
+  <si>
+    <t>nachos</t>
   </si>
 </sst>
 </file>
@@ -2475,7 +2475,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2617,9 +2617,6 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2694,6 +2691,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3858,8 +3885,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:AG73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4008,7 +4035,7 @@
       </c>
     </row>
     <row r="8" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="74" t="s">
         <v>389</v>
       </c>
       <c r="C8" s="35"/>
@@ -4017,7 +4044,7 @@
       <c r="F8" s="49"/>
     </row>
     <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="61" t="s">
         <v>284</v>
       </c>
       <c r="C9" s="45"/>
@@ -4026,7 +4053,7 @@
       <c r="F9" s="49"/>
     </row>
     <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="62" t="s">
         <v>285</v>
       </c>
       <c r="C10" s="46"/>
@@ -4035,7 +4062,7 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="63" t="s">
         <v>286</v>
       </c>
       <c r="C11" s="47"/>
@@ -4044,7 +4071,7 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="60" t="s">
         <v>282</v>
       </c>
       <c r="C12" s="35"/>
@@ -4053,7 +4080,7 @@
       <c r="F12" s="49"/>
     </row>
     <row r="13" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="60" t="s">
         <v>283</v>
       </c>
       <c r="C13" s="35"/>
@@ -4062,7 +4089,7 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="74" t="s">
         <v>390</v>
       </c>
       <c r="C14" s="35"/>
@@ -4071,7 +4098,7 @@
       <c r="F14" s="49"/>
     </row>
     <row r="15" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="74" t="s">
         <v>391</v>
       </c>
       <c r="C15" s="35"/>
@@ -4080,7 +4107,7 @@
       <c r="F15" s="49"/>
     </row>
     <row r="16" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="60" t="s">
         <v>287</v>
       </c>
       <c r="C16" s="35"/>
@@ -4089,7 +4116,7 @@
       <c r="F16" s="49"/>
     </row>
     <row r="17" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>392</v>
       </c>
       <c r="C17" s="35"/>
@@ -4098,7 +4125,7 @@
       <c r="F17" s="49"/>
     </row>
     <row r="18" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="64" t="s">
         <v>288</v>
       </c>
       <c r="C18" s="35"/>
@@ -4151,65 +4178,65 @@
       </c>
     </row>
     <row r="23" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="73" t="s">
         <v>371</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="53" t="s">
-        <v>434</v>
+      <c r="D23" s="53">
+        <v>1004</v>
       </c>
       <c r="E23" s="48"/>
       <c r="G23" s="36"/>
     </row>
     <row r="24" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="73" t="s">
         <v>372</v>
       </c>
       <c r="C24" s="35"/>
-      <c r="D24" s="53" t="s">
-        <v>436</v>
+      <c r="D24" s="81" t="s">
+        <v>428</v>
       </c>
       <c r="E24" s="35"/>
     </row>
     <row r="25" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="73" t="s">
         <v>373</v>
       </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="54" t="s">
-        <v>440</v>
+      <c r="D25" s="82" t="s">
+        <v>429</v>
       </c>
       <c r="E25" s="35"/>
     </row>
     <row r="26" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="74" t="s">
         <v>395</v>
       </c>
       <c r="C26" s="35"/>
-      <c r="D26" s="53" t="s">
-        <v>438</v>
+      <c r="D26" s="81" t="s">
+        <v>430</v>
       </c>
       <c r="E26" s="48"/>
       <c r="G26" s="36"/>
     </row>
     <row r="27" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="73" t="s">
         <v>374</v>
       </c>
       <c r="C27" s="35"/>
-      <c r="D27" s="53" t="s">
-        <v>439</v>
+      <c r="D27" s="81" t="s">
+        <v>431</v>
       </c>
       <c r="E27" s="48"/>
       <c r="G27" s="36"/>
     </row>
     <row r="28" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="75" t="s">
         <v>396</v>
       </c>
       <c r="C28" s="35"/>
-      <c r="D28" s="55" t="s">
-        <v>435</v>
+      <c r="D28" s="54">
+        <v>45955</v>
       </c>
       <c r="E28" s="48"/>
       <c r="F28" s="49"/>
@@ -4260,49 +4287,57 @@
       </c>
     </row>
     <row r="32" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B32" s="77" t="s">
+      <c r="B32" s="76" t="s">
         <v>375</v>
       </c>
       <c r="C32" s="49"/>
-      <c r="D32" s="56">
-        <v>1004</v>
+      <c r="D32" s="55">
+        <v>1234</v>
       </c>
       <c r="E32" s="50"/>
       <c r="G32" s="36"/>
     </row>
     <row r="33" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B33" s="77" t="s">
+      <c r="B33" s="76" t="s">
         <v>376</v>
       </c>
       <c r="C33" s="50"/>
-      <c r="D33" s="56"/>
+      <c r="D33" s="54">
+        <v>45955</v>
+      </c>
       <c r="E33" s="50"/>
       <c r="G33" s="36"/>
     </row>
     <row r="34" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B34" s="77" t="s">
+      <c r="B34" s="76" t="s">
         <v>377</v>
       </c>
       <c r="C34" s="49"/>
-      <c r="D34" s="56"/>
+      <c r="D34" s="55">
+        <v>12345</v>
+      </c>
       <c r="E34" s="50"/>
       <c r="G34" s="36"/>
     </row>
     <row r="35" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="76" t="s">
         <v>393</v>
       </c>
       <c r="C35" s="49"/>
-      <c r="D35" s="56"/>
+      <c r="D35" s="81" t="s">
+        <v>432</v>
+      </c>
       <c r="E35" s="50"/>
       <c r="G35" s="36"/>
     </row>
     <row r="36" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B36" s="77" t="s">
+      <c r="B36" s="76" t="s">
         <v>394</v>
       </c>
       <c r="C36" s="49"/>
-      <c r="D36" s="56"/>
+      <c r="D36" s="55">
+        <v>123456</v>
+      </c>
       <c r="E36" s="50"/>
       <c r="G36" s="36"/>
     </row>
@@ -4351,11 +4386,13 @@
       </c>
     </row>
     <row r="40" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B40" s="81" t="s">
+      <c r="B40" s="80" t="s">
         <v>427</v>
       </c>
       <c r="C40" s="49"/>
-      <c r="D40" s="57"/>
+      <c r="D40" s="56">
+        <v>36892</v>
+      </c>
       <c r="E40" s="37"/>
       <c r="G40" s="36"/>
     </row>
@@ -4364,16 +4401,18 @@
         <v>378</v>
       </c>
       <c r="C41" s="50"/>
-      <c r="D41" s="56"/>
+      <c r="D41" s="55">
+        <v>0.255</v>
+      </c>
       <c r="G41" s="36"/>
     </row>
     <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="77" t="s">
+      <c r="B42" s="76" t="s">
         <v>333</v>
       </c>
       <c r="C42" s="50"/>
       <c r="D42" s="42" t="s">
-        <v>431</v>
+        <v>334</v>
       </c>
       <c r="G42" s="36"/>
     </row>
@@ -4382,7 +4421,9 @@
         <v>303</v>
       </c>
       <c r="C43" s="50"/>
-      <c r="D43" s="56"/>
+      <c r="D43" s="84">
+        <v>45713</v>
+      </c>
       <c r="G43" s="36"/>
     </row>
     <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
@@ -4434,18 +4475,22 @@
       <c r="B47" s="38" t="s">
         <v>379</v>
       </c>
-      <c r="D47" s="56"/>
+      <c r="D47" s="83" t="s">
+        <v>433</v>
+      </c>
       <c r="G47" s="36"/>
       <c r="AG47" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:33" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="57" t="s">
         <v>343</v>
       </c>
       <c r="C48" s="30"/>
-      <c r="D48" s="56"/>
+      <c r="D48" s="83" t="s">
+        <v>434</v>
+      </c>
       <c r="E48" s="30"/>
       <c r="G48" s="36"/>
     </row>
@@ -4454,7 +4499,9 @@
         <v>344</v>
       </c>
       <c r="C49" s="30"/>
-      <c r="D49" s="56"/>
+      <c r="D49" s="83" t="s">
+        <v>435</v>
+      </c>
       <c r="E49" s="30"/>
       <c r="G49" s="36"/>
     </row>
@@ -4464,7 +4511,7 @@
       </c>
       <c r="C50" s="50"/>
       <c r="D50" s="42" t="s">
-        <v>433</v>
+        <v>12</v>
       </c>
       <c r="G50" s="36"/>
     </row>
@@ -4474,7 +4521,7 @@
       </c>
       <c r="C51" s="50"/>
       <c r="D51" s="42" t="s">
-        <v>432</v>
+        <v>186</v>
       </c>
       <c r="G51" s="36"/>
     </row>
@@ -4483,34 +4530,36 @@
         <v>380</v>
       </c>
       <c r="C52" s="50"/>
-      <c r="D52" s="66"/>
+      <c r="D52" s="65">
+        <v>132.5</v>
+      </c>
       <c r="G52" s="36"/>
     </row>
     <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="81" t="s">
+      <c r="B53" s="80" t="s">
         <v>426</v>
       </c>
       <c r="C53" s="50"/>
       <c r="D53" s="43" t="s">
-        <v>428</v>
+        <v>180</v>
       </c>
       <c r="G53" s="36"/>
     </row>
     <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" s="77" t="s">
+      <c r="B54" s="76" t="s">
         <v>318</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>429</v>
+        <v>180</v>
       </c>
       <c r="G54" s="36"/>
     </row>
     <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="77" t="s">
+      <c r="B55" s="76" t="s">
         <v>319</v>
       </c>
       <c r="D55" s="44" t="s">
-        <v>430</v>
+        <v>181</v>
       </c>
       <c r="G55" s="36"/>
     </row>
@@ -4518,7 +4567,9 @@
       <c r="B56" s="38" t="s">
         <v>370</v>
       </c>
-      <c r="D56" s="66"/>
+      <c r="D56" s="65">
+        <v>123.98699999999999</v>
+      </c>
       <c r="G56" s="36"/>
     </row>
     <row r="57" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
@@ -4566,63 +4617,75 @@
       </c>
     </row>
     <row r="60" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B60" s="77" t="s">
+      <c r="B60" s="76" t="s">
         <v>381</v>
       </c>
-      <c r="D60" s="66"/>
+      <c r="D60" s="65">
+        <v>42</v>
+      </c>
       <c r="G60" s="36"/>
     </row>
     <row r="61" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="B61" s="77" t="s">
+      <c r="B61" s="76" t="s">
         <v>382</v>
       </c>
-      <c r="D61" s="57"/>
+      <c r="D61" s="85" t="s">
+        <v>436</v>
+      </c>
       <c r="G61" s="36"/>
     </row>
     <row r="62" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B62" s="38" t="s">
         <v>383</v>
       </c>
-      <c r="D62" s="57"/>
+      <c r="D62" s="85" t="s">
+        <v>437</v>
+      </c>
       <c r="G62" s="36"/>
     </row>
     <row r="63" spans="2:33" s="20" customFormat="1" ht="15.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="38" t="s">
         <v>384</v>
       </c>
-      <c r="D63" s="56"/>
+      <c r="D63" s="86" t="s">
+        <v>438</v>
+      </c>
       <c r="G63" s="36"/>
     </row>
     <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B64" s="77" t="s">
+      <c r="B64" s="76" t="s">
         <v>315</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>437</v>
+        <v>10</v>
       </c>
       <c r="G64" s="36"/>
     </row>
     <row r="65" spans="2:7" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B65" s="77" t="s">
+      <c r="B65" s="76" t="s">
         <v>397</v>
       </c>
-      <c r="D65" s="66"/>
+      <c r="D65" s="87">
+        <v>42060</v>
+      </c>
       <c r="G65" s="36"/>
     </row>
     <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B66" s="77" t="s">
+      <c r="B66" s="76" t="s">
         <v>316</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>441</v>
+        <v>164</v>
       </c>
       <c r="G66" s="36"/>
     </row>
     <row r="67" spans="2:7" s="20" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="B67" s="77" t="s">
+      <c r="B67" s="76" t="s">
         <v>398</v>
       </c>
-      <c r="D67" s="66"/>
+      <c r="D67" s="65">
+        <v>15</v>
+      </c>
       <c r="G67" s="36"/>
     </row>
     <row r="68" spans="2:7" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
@@ -4634,17 +4697,21 @@
     </row>
     <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.5"/>
     <row r="71" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B71" s="77" t="s">
+      <c r="B71" s="76" t="s">
         <v>385</v>
       </c>
-      <c r="D71" s="57"/>
+      <c r="D71" s="88" t="s">
+        <v>439</v>
+      </c>
       <c r="G71" s="36"/>
     </row>
     <row r="72" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
-      <c r="B72" s="77" t="s">
+      <c r="B72" s="76" t="s">
         <v>386</v>
       </c>
-      <c r="D72" s="57"/>
+      <c r="D72" s="88" t="s">
+        <v>440</v>
+      </c>
       <c r="G72" s="36"/>
     </row>
     <row r="73" spans="2:7" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
@@ -4652,11 +4719,12 @@
         <v>425</v>
       </c>
       <c r="C73" s="41"/>
-      <c r="D73" s="66"/>
+      <c r="D73" s="83" t="s">
+        <v>441</v>
+      </c>
       <c r="G73" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Nxmx14c/xh/1eCFWGRpZm4SQG3n0jL7dP8UexS5j75+YdBcRD4u7dyGUABbveoNs4LfpbnTze5LpASDK+PFtng==" saltValue="zjcfnmik8tk9YV1sHAXvOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D42">
     <cfRule type="expression" dxfId="13" priority="11">
       <formula xml:space="preserve"> IF(LEFT($D$42, 13)="Please Select", TRUE)</formula>
@@ -6412,7 +6480,7 @@
         <f t="shared" ref="F88:F89" si="5">$B$13</f>
         <v>Resolved</v>
       </c>
-      <c r="G88" s="59" t="s">
+      <c r="G88" s="58" t="s">
         <v>338</v>
       </c>
     </row>
@@ -6433,7 +6501,7 @@
         <f t="shared" si="5"/>
         <v>Resolved</v>
       </c>
-      <c r="G89" s="59" t="s">
+      <c r="G89" s="58" t="s">
         <v>419</v>
       </c>
     </row>
@@ -6475,13 +6543,13 @@
         <f t="shared" si="6"/>
         <v>Resolved</v>
       </c>
-      <c r="G91" s="59"/>
+      <c r="G91" s="58"/>
     </row>
     <row r="92" spans="2:7" s="20" customFormat="1" ht="186.35" x14ac:dyDescent="0.5">
       <c r="B92" s="20">
         <v>71</v>
       </c>
-      <c r="C92" s="60" t="s">
+      <c r="C92" s="59" t="s">
         <v>278</v>
       </c>
       <c r="D92" s="24">
@@ -7065,8 +7133,8 @@
     <col min="6" max="17" width="16.703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B2" s="71" t="s">
+    <row r="2" spans="1:17" s="70" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B2" s="70" t="s">
         <v>158</v>
       </c>
     </row>
@@ -7141,8 +7209,8 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B8" s="72" t="s">
+    <row r="8" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B8" s="71" t="s">
         <v>363</v>
       </c>
     </row>
@@ -7169,17 +7237,17 @@
       <c r="E10" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
@@ -7187,7 +7255,7 @@
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDIRECT(B11)</f>
-        <v>{{ emission_identified_flag_fk }}</v>
+        <v>Operator was aware of the leak prior to receiving the CARB plume notification</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">INDIRECT("'" &amp; CELL("filename", INDIRECT(B11)) &amp; "'!" &amp; ADDRESS(ROW(INDIRECT(B11)), COLUMN(INDIRECT(B11)) - 2))</f>
@@ -7201,7 +7269,7 @@
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT(B12)</f>
-        <v>{{ emission_type_fk }}</v>
+        <v>An unintentional leak  (i.e., the operator was not aware of, and could be repaired if discovered)</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">INDIRECT("'" &amp; CELL("filename", INDIRECT(B12)) &amp; "'!" &amp; ADDRESS(ROW(INDIRECT(B12)), COLUMN(INDIRECT(B12)) - 2))</f>
@@ -7215,7 +7283,7 @@
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDIRECT(B13)</f>
-        <v>{{ emission_location }}</v>
+        <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">INDIRECT("'" &amp; CELL("filename", INDIRECT(B13)) &amp; "'!" &amp; ADDRESS(ROW(INDIRECT(B13)), COLUMN(INDIRECT(B13)) - 2))</f>
@@ -7223,8 +7291,8 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="15" spans="1:17" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B15" s="72" t="s">
+    <row r="15" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B15" s="71" t="s">
         <v>364</v>
       </c>
     </row>
@@ -7443,7 +7511,7 @@
       </c>
     </row>
     <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B48" s="67" t="str" cm="1">
+      <c r="B48" s="66" t="str" cm="1">
         <f t="array" ref="B48:B58">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.TOCOL(C64:M70, 1)))</f>
         <v>Collection system downtime</v>
       </c>
@@ -7451,70 +7519,70 @@
       <c r="Q48"/>
     </row>
     <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B49" s="69" t="str">
+      <c r="B49" s="68" t="str">
         <v>Construction - New Well Installation</v>
       </c>
       <c r="E49" s="7"/>
       <c r="Q49"/>
     </row>
     <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B50" s="70" t="str">
+      <c r="B50" s="69" t="str">
         <v>Construction - Well Raising or Horizontal Extension</v>
       </c>
       <c r="E50" s="7"/>
       <c r="Q50"/>
     </row>
     <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B51" s="68" t="str">
+      <c r="B51" s="67" t="str">
         <v>Cover integrity</v>
       </c>
       <c r="E51" s="7"/>
       <c r="Q51"/>
     </row>
     <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B52" s="67" t="str">
+      <c r="B52" s="66" t="str">
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
       <c r="E52" s="7"/>
       <c r="Q52"/>
     </row>
     <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B53" s="68" t="str">
+      <c r="B53" s="67" t="str">
         <v>Cracked/Broken Seal</v>
       </c>
       <c r="E53" s="7"/>
       <c r="Q53"/>
     </row>
     <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B54" s="67" t="str">
+      <c r="B54" s="66" t="str">
         <v>Damaged component</v>
       </c>
       <c r="E54" s="7"/>
       <c r="Q54"/>
     </row>
     <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B55" s="67" t="str">
+      <c r="B55" s="66" t="str">
         <v>Insufficient vacuum</v>
       </c>
       <c r="E55" s="7"/>
       <c r="Q55"/>
     </row>
     <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B56" s="69" t="str">
+      <c r="B56" s="68" t="str">
         <v>Offline Gas Collection Well(s)</v>
       </c>
       <c r="E56" s="7"/>
       <c r="Q56"/>
     </row>
     <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B57" s="70" t="str">
+      <c r="B57" s="69" t="str">
         <v>Other</v>
       </c>
       <c r="E57" s="7"/>
       <c r="Q57"/>
     </row>
     <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B58" s="68" t="str">
+      <c r="B58" s="67" t="str">
         <v>Uncontrolled Area (no gas collection infrastructure)</v>
       </c>
       <c r="E58" s="7"/>
@@ -8245,8 +8313,8 @@
     <row r="134" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G134"/>
     </row>
-    <row r="135" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B135" s="72" t="s">
+    <row r="135" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B135" s="71" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8308,8 +8376,8 @@
     <row r="143" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G143"/>
     </row>
-    <row r="144" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B144" s="72" t="s">
+    <row r="144" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B144" s="71" t="s">
         <v>366</v>
       </c>
     </row>
@@ -8391,8 +8459,8 @@
     <row r="154" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G154"/>
     </row>
-    <row r="155" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B155" s="72" t="s">
+    <row r="155" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B155" s="71" t="s">
         <v>367</v>
       </c>
     </row>
@@ -8504,8 +8572,8 @@
     <row r="168" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G168"/>
     </row>
-    <row r="169" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B169" s="72" t="s">
+    <row r="169" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B169" s="71" t="s">
         <v>368</v>
       </c>
     </row>
@@ -8531,7 +8599,7 @@
         <v>163</v>
       </c>
       <c r="C173" t="str" cm="1">
-        <f t="array" aca="1" ref="C173" ca="1">_xlfn._xlws.FILTER($B$173:$B$189,$B$173:$B$189 &lt;&gt; "")</f>
+        <f t="array" aca="1" ref="C173:C180" ca="1">_xlfn._xlws.FILTER($B$173:$B$189,$B$173:$B$189 &lt;&gt; "")</f>
         <v>Please Select</v>
       </c>
       <c r="G173"/>
@@ -8541,31 +8609,83 @@
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
       </c>
+      <c r="C174" t="str">
+        <f ca="1"/>
+        <v>Offline Gas Collection Well(s)</v>
+      </c>
       <c r="G174"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B175" t="str" cm="1">
-        <f t="array" aca="1" ref="B175" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
-        <v/>
+        <f t="array" aca="1" ref="B175:B181" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
+        <v>Offline Gas Collection Well(s)</v>
+      </c>
+      <c r="C175" t="str">
+        <f ca="1"/>
+        <v>Construction - New Well Installation</v>
       </c>
       <c r="G175"/>
     </row>
     <row r="176" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B176" t="str">
+        <f ca="1"/>
+        <v>Construction - New Well Installation</v>
+      </c>
+      <c r="C176" t="str">
+        <f ca="1"/>
+        <v>Construction - Well Raising or Horizontal Extension</v>
+      </c>
       <c r="G176"/>
     </row>
     <row r="177" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B177" t="str">
+        <f ca="1"/>
+        <v>Construction - Well Raising or Horizontal Extension</v>
+      </c>
+      <c r="C177" t="str">
+        <f ca="1"/>
+        <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
+      </c>
       <c r="G177"/>
     </row>
     <row r="178" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B178" t="str">
+        <f ca="1"/>
+        <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
+      </c>
+      <c r="C178" t="str">
+        <f ca="1"/>
+        <v>Damaged component</v>
+      </c>
       <c r="G178"/>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B179" t="str">
+        <f ca="1"/>
+        <v>Damaged component</v>
+      </c>
+      <c r="C179" t="str">
+        <f ca="1"/>
+        <v>Insufficient vacuum</v>
+      </c>
       <c r="G179"/>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B180" t="str">
+        <f ca="1"/>
+        <v>Insufficient vacuum</v>
+      </c>
+      <c r="C180" t="str">
+        <f ca="1"/>
+        <v>Other</v>
+      </c>
       <c r="G180"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B181" t="str">
+        <f ca="1"/>
+        <v>Other</v>
+      </c>
       <c r="G181"/>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.5">
@@ -8595,8 +8715,8 @@
     <row r="190" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G190"/>
     </row>
-    <row r="191" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B191" s="72" t="s">
+    <row r="191" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B191" s="71" t="s">
         <v>369</v>
       </c>
     </row>
@@ -8622,7 +8742,7 @@
         <v>163</v>
       </c>
       <c r="C195" t="str" cm="1">
-        <f t="array" aca="1" ref="C195:C196" ca="1">_xlfn._xlws.FILTER($B$195:$B$211,$B$195:$B$211 &lt;&gt; "")</f>
+        <f t="array" aca="1" ref="C195:C203" ca="1">_xlfn._xlws.FILTER($B$195:$B$211,$B$195:$B$211 &lt;&gt; "")</f>
         <v>Please Select</v>
       </c>
       <c r="G195"/>
@@ -8642,31 +8762,83 @@
       <c r="B197" t="s">
         <v>355</v>
       </c>
+      <c r="C197" t="str">
+        <f ca="1"/>
+        <v>Offline Gas Collection Well(s)</v>
+      </c>
       <c r="G197"/>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B198" t="str" cm="1">
-        <f t="array" aca="1" ref="B198" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
-        <v/>
+        <f t="array" aca="1" ref="B198:B204" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
+        <v>Offline Gas Collection Well(s)</v>
+      </c>
+      <c r="C198" t="str">
+        <f ca="1"/>
+        <v>Construction - New Well Installation</v>
       </c>
       <c r="G198"/>
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B199" t="str">
+        <f ca="1"/>
+        <v>Construction - New Well Installation</v>
+      </c>
+      <c r="C199" t="str">
+        <f ca="1"/>
+        <v>Construction - Well Raising or Horizontal Extension</v>
+      </c>
       <c r="G199"/>
     </row>
     <row r="200" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B200" t="str">
+        <f ca="1"/>
+        <v>Construction - Well Raising or Horizontal Extension</v>
+      </c>
+      <c r="C200" t="str">
+        <f ca="1"/>
+        <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
+      </c>
       <c r="G200"/>
     </row>
     <row r="201" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B201" t="str">
+        <f ca="1"/>
+        <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
+      </c>
+      <c r="C201" t="str">
+        <f ca="1"/>
+        <v>Damaged component</v>
+      </c>
       <c r="G201"/>
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B202" t="str">
+        <f ca="1"/>
+        <v>Damaged component</v>
+      </c>
+      <c r="C202" t="str">
+        <f ca="1"/>
+        <v>Insufficient vacuum</v>
+      </c>
       <c r="G202"/>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B203" t="str">
+        <f ca="1"/>
+        <v>Insufficient vacuum</v>
+      </c>
+      <c r="C203" t="str">
+        <f ca="1"/>
+        <v>Other</v>
+      </c>
       <c r="G203"/>
     </row>
     <row r="204" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B204" t="str">
+        <f ca="1"/>
+        <v>Other</v>
+      </c>
       <c r="G204"/>
     </row>
     <row r="205" spans="2:7" x14ac:dyDescent="0.5">
@@ -8687,8 +8859,8 @@
     <row r="210" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G210"/>
     </row>
-    <row r="213" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="B213" s="72" t="s">
+    <row r="213" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B213" s="71" t="s">
         <v>365</v>
       </c>
     </row>
@@ -9674,322 +9846,322 @@
       <c r="F2" s="25"/>
     </row>
     <row r="6" spans="2:13" ht="86" x14ac:dyDescent="0.5">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="77" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="77" t="s">
         <v>407</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="78" t="s">
         <v>408</v>
       </c>
-      <c r="E6" s="78" t="s">
+      <c r="E6" s="77" t="s">
         <v>409</v>
       </c>
-      <c r="F6" s="78" t="s">
+      <c r="F6" s="77" t="s">
         <v>410</v>
       </c>
-      <c r="G6" s="78" t="s">
+      <c r="G6" s="77" t="s">
         <v>411</v>
       </c>
-      <c r="H6" s="78" t="s">
+      <c r="H6" s="77" t="s">
         <v>412</v>
       </c>
-      <c r="I6" s="78" t="s">
+      <c r="I6" s="77" t="s">
         <v>413</v>
       </c>
-      <c r="J6" s="78" t="s">
+      <c r="J6" s="77" t="s">
         <v>414</v>
       </c>
-      <c r="K6" s="78" t="s">
+      <c r="K6" s="77" t="s">
         <v>415</v>
       </c>
-      <c r="L6" s="78" t="s">
+      <c r="L6" s="77" t="s">
         <v>416</v>
       </c>
-      <c r="M6" s="78" t="s">
+      <c r="M6" s="77" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="80"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="80"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="80"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="80"/>
-      <c r="M20" s="80"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="80"/>
-      <c r="M21" s="80"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="79"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="80"/>
-      <c r="M23" s="80"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="80"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.5">
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="VwJlKEdUa2d6FHnYCytBv5G8UoZUdgoWcJGdel8EpnF4T15YAfRvfoWRk2Fzdvvss+vBp+oQZtzTB2RAg6gCmg==" saltValue="NkJG9DFU1K/CmFoOV2bKyw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -9998,14 +10170,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10244,21 +10414,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10283,9 +10452,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updating portal change logging
</commit_message>
<xml_diff>
--- a/feedback_forms/testing_versions/landfill_operator_feedback_v070_with_errors_02.xlsx
+++ b/feedback_forms/testing_versions/landfill_operator_feedback_v070_with_errors_02.xlsx
@@ -11,7 +11,7 @@
   <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{0BB98C50-23F5-43F3-BCBC-FF70E147074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA690751-B54B-4DA8-9261-F1EFC560B0E3}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="vY3M817KAomZyhlm4oS6cOyuUSxWaTaz7lVX62BALQGX5cCDz411RVbfnvbnpvf21HlxJBaGYtmscNkzHgnKag==" workbookSaltValue="+DW2WdW8uRq+VBPkAiodVA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4547" yWindow="2500" windowWidth="19200" windowHeight="11093" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="1350" yWindow="840" windowWidth="23730" windowHeight="14025" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -2084,13 +2084,19 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2472,50 +2478,50 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2523,8 +2529,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2533,127 +2539,127 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2665,10 +2671,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2676,10 +2685,7 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2689,32 +2695,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3886,20 +3892,20 @@
   <dimension ref="B1:AG73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1171875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="65.703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="4.703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="65.703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="4.1171875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" style="19" customWidth="1"/>
     <col min="6" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -3935,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
@@ -3944,7 +3950,7 @@
       <c r="E2" s="31"/>
       <c r="F2" s="49"/>
     </row>
-    <row r="3" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
@@ -3953,13 +3959,13 @@
       <c r="E3" s="31"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="2:33" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:33" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -3995,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
@@ -4029,12 +4035,12 @@
       <c r="AF6" s="52"/>
       <c r="AG6" s="52"/>
     </row>
-    <row r="7" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG7" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="74" t="s">
         <v>389</v>
       </c>
@@ -4043,7 +4049,7 @@
       <c r="E8" s="35"/>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="61" t="s">
         <v>284</v>
       </c>
@@ -4052,7 +4058,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="49"/>
     </row>
-    <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="62" t="s">
         <v>285</v>
       </c>
@@ -4061,7 +4067,7 @@
       <c r="E10" s="35"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="63" t="s">
         <v>286</v>
       </c>
@@ -4070,7 +4076,7 @@
       <c r="E11" s="35"/>
       <c r="F11" s="49"/>
     </row>
-    <row r="12" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="60" t="s">
         <v>282</v>
       </c>
@@ -4079,7 +4085,7 @@
       <c r="E12" s="35"/>
       <c r="F12" s="49"/>
     </row>
-    <row r="13" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="60" t="s">
         <v>283</v>
       </c>
@@ -4088,7 +4094,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="49"/>
     </row>
-    <row r="14" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="74" t="s">
         <v>390</v>
       </c>
@@ -4097,7 +4103,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="49"/>
     </row>
-    <row r="15" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="74" t="s">
         <v>391</v>
       </c>
@@ -4106,7 +4112,7 @@
       <c r="E15" s="35"/>
       <c r="F15" s="49"/>
     </row>
-    <row r="16" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="60" t="s">
         <v>287</v>
       </c>
@@ -4115,7 +4121,7 @@
       <c r="E16" s="35"/>
       <c r="F16" s="49"/>
     </row>
-    <row r="17" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="74" t="s">
         <v>392</v>
       </c>
@@ -4124,7 +4130,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="49"/>
     </row>
-    <row r="18" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="64" t="s">
         <v>288</v>
       </c>
@@ -4133,12 +4139,12 @@
       <c r="E18" s="35"/>
       <c r="F18" s="49"/>
     </row>
-    <row r="20" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG20" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51"/>
@@ -4172,12 +4178,12 @@
       <c r="AF21" s="52"/>
       <c r="AG21" s="52"/>
     </row>
-    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG22" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="73" t="s">
         <v>371</v>
       </c>
@@ -4188,7 +4194,7 @@
       <c r="E23" s="48"/>
       <c r="G23" s="36"/>
     </row>
-    <row r="24" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="73" t="s">
         <v>372</v>
       </c>
@@ -4198,7 +4204,7 @@
       </c>
       <c r="E24" s="35"/>
     </row>
-    <row r="25" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="73" t="s">
         <v>373</v>
       </c>
@@ -4208,7 +4214,7 @@
       </c>
       <c r="E25" s="35"/>
     </row>
-    <row r="26" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="74" t="s">
         <v>395</v>
       </c>
@@ -4219,7 +4225,7 @@
       <c r="E26" s="48"/>
       <c r="G26" s="36"/>
     </row>
-    <row r="27" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="73" t="s">
         <v>374</v>
       </c>
@@ -4230,7 +4236,7 @@
       <c r="E27" s="48"/>
       <c r="G27" s="36"/>
     </row>
-    <row r="28" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="75" t="s">
         <v>396</v>
       </c>
@@ -4242,12 +4248,12 @@
       <c r="F28" s="49"/>
       <c r="G28" s="36"/>
     </row>
-    <row r="29" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG29" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="51"/>
@@ -4281,12 +4287,12 @@
       <c r="AF30" s="52"/>
       <c r="AG30" s="52"/>
     </row>
-    <row r="31" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG31" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="76" t="s">
         <v>375</v>
       </c>
@@ -4297,7 +4303,7 @@
       <c r="E32" s="50"/>
       <c r="G32" s="36"/>
     </row>
-    <row r="33" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="76" t="s">
         <v>376</v>
       </c>
@@ -4308,7 +4314,7 @@
       <c r="E33" s="50"/>
       <c r="G33" s="36"/>
     </row>
-    <row r="34" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="76" t="s">
         <v>377</v>
       </c>
@@ -4319,7 +4325,7 @@
       <c r="E34" s="50"/>
       <c r="G34" s="36"/>
     </row>
-    <row r="35" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="76" t="s">
         <v>393</v>
       </c>
@@ -4330,7 +4336,7 @@
       <c r="E35" s="50"/>
       <c r="G35" s="36"/>
     </row>
-    <row r="36" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="76" t="s">
         <v>394</v>
       </c>
@@ -4341,12 +4347,12 @@
       <c r="E36" s="50"/>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG37" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
       <c r="D38" s="51"/>
@@ -4380,12 +4386,12 @@
       <c r="AF38" s="52"/>
       <c r="AG38" s="52"/>
     </row>
-    <row r="39" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG39" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="80" t="s">
         <v>427</v>
       </c>
@@ -4396,7 +4402,7 @@
       <c r="E40" s="37"/>
       <c r="G40" s="36"/>
     </row>
-    <row r="41" spans="2:33" s="20" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:33" s="20" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="38" t="s">
         <v>378</v>
       </c>
@@ -4406,7 +4412,7 @@
       </c>
       <c r="G41" s="36"/>
     </row>
-    <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="76" t="s">
         <v>333</v>
       </c>
@@ -4416,7 +4422,7 @@
       </c>
       <c r="G42" s="36"/>
     </row>
-    <row r="43" spans="2:33" s="20" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:33" s="20" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B43" s="38" t="s">
         <v>303</v>
       </c>
@@ -4426,12 +4432,12 @@
       </c>
       <c r="G43" s="36"/>
     </row>
-    <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG44" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
@@ -4465,13 +4471,13 @@
       <c r="AF45" s="52"/>
       <c r="AG45" s="52"/>
     </row>
-    <row r="46" spans="2:33" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="49"/>
       <c r="AG46" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:33" s="30" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:33" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="38" t="s">
         <v>379</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:33" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:33" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B48" s="57" t="s">
         <v>343</v>
       </c>
@@ -4494,7 +4500,7 @@
       <c r="E48" s="30"/>
       <c r="G48" s="36"/>
     </row>
-    <row r="49" spans="2:33" s="20" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:33" s="20" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="38" t="s">
         <v>344</v>
       </c>
@@ -4505,7 +4511,7 @@
       <c r="E49" s="30"/>
       <c r="G49" s="36"/>
     </row>
-    <row r="50" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="38" t="s">
         <v>359</v>
       </c>
@@ -4515,7 +4521,7 @@
       </c>
       <c r="G50" s="36"/>
     </row>
-    <row r="51" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="38" t="s">
         <v>361</v>
       </c>
@@ -4525,7 +4531,7 @@
       </c>
       <c r="G51" s="36"/>
     </row>
-    <row r="52" spans="2:33" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:33" s="20" customFormat="1" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="38" t="s">
         <v>380</v>
       </c>
@@ -4535,7 +4541,7 @@
       </c>
       <c r="G52" s="36"/>
     </row>
-    <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="80" t="s">
         <v>426</v>
       </c>
@@ -4545,7 +4551,7 @@
       </c>
       <c r="G53" s="36"/>
     </row>
-    <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="76" t="s">
         <v>318</v>
       </c>
@@ -4554,7 +4560,7 @@
       </c>
       <c r="G54" s="36"/>
     </row>
-    <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="76" t="s">
         <v>319</v>
       </c>
@@ -4563,7 +4569,7 @@
       </c>
       <c r="G55" s="36"/>
     </row>
-    <row r="56" spans="2:33" s="20" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:33" s="20" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B56" s="38" t="s">
         <v>370</v>
       </c>
@@ -4572,12 +4578,12 @@
       </c>
       <c r="G56" s="36"/>
     </row>
-    <row r="57" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
       <c r="D57" s="50"/>
     </row>
-    <row r="58" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
       <c r="D58" s="51"/>
@@ -4611,12 +4617,12 @@
       <c r="AF58" s="52"/>
       <c r="AG58" s="52"/>
     </row>
-    <row r="59" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG59" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="76" t="s">
         <v>381</v>
       </c>
@@ -4625,7 +4631,7 @@
       </c>
       <c r="G60" s="36"/>
     </row>
-    <row r="61" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="76" t="s">
         <v>382</v>
       </c>
@@ -4634,7 +4640,7 @@
       </c>
       <c r="G61" s="36"/>
     </row>
-    <row r="62" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="38" t="s">
         <v>383</v>
       </c>
@@ -4643,7 +4649,7 @@
       </c>
       <c r="G62" s="36"/>
     </row>
-    <row r="63" spans="2:33" s="20" customFormat="1" ht="15.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:33" s="20" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="38" t="s">
         <v>384</v>
       </c>
@@ -4652,7 +4658,7 @@
       </c>
       <c r="G63" s="36"/>
     </row>
-    <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="76" t="s">
         <v>315</v>
       </c>
@@ -4661,7 +4667,7 @@
       </c>
       <c r="G64" s="36"/>
     </row>
-    <row r="65" spans="2:7" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:7" s="20" customFormat="1" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="76" t="s">
         <v>397</v>
       </c>
@@ -4670,7 +4676,7 @@
       </c>
       <c r="G65" s="36"/>
     </row>
-    <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="76" t="s">
         <v>316</v>
       </c>
@@ -4679,7 +4685,7 @@
       </c>
       <c r="G66" s="36"/>
     </row>
-    <row r="67" spans="2:7" s="20" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:7" s="20" customFormat="1" ht="31.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B67" s="76" t="s">
         <v>398</v>
       </c>
@@ -4688,15 +4694,15 @@
       </c>
       <c r="G67" s="36"/>
     </row>
-    <row r="68" spans="2:7" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="50"/>
       <c r="D68" s="39"/>
     </row>
-    <row r="69" spans="2:7" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:7" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G69" s="36"/>
     </row>
-    <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="71" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:7" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B71" s="76" t="s">
         <v>385</v>
       </c>
@@ -4705,7 +4711,7 @@
       </c>
       <c r="G71" s="36"/>
     </row>
-    <row r="72" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:7" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B72" s="76" t="s">
         <v>386</v>
       </c>
@@ -4714,7 +4720,7 @@
       </c>
       <c r="G72" s="36"/>
     </row>
-    <row r="73" spans="2:7" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:7" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="38" t="s">
         <v>425</v>
       </c>
@@ -4889,18 +4895,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="45.703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:18" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>14</v>
       </c>
@@ -4908,7 +4914,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G3" s="4"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -4922,7 +4928,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4930,15 +4936,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -4946,7 +4952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>20</v>
       </c>
@@ -4957,7 +4963,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>22</v>
       </c>
@@ -4968,7 +4974,7 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>24</v>
       </c>
@@ -4979,7 +4985,7 @@
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>26</v>
       </c>
@@ -4990,15 +4996,15 @@
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
       <c r="C14" s="23"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="20"/>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
@@ -5015,7 +5021,7 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -5029,7 +5035,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -5060,7 +5066,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="2:18" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:18" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>1</v>
       </c>
@@ -5081,7 +5087,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="20">
         <v>2</v>
       </c>
@@ -5102,7 +5108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <v>3</v>
       </c>
@@ -5123,7 +5129,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <v>4</v>
       </c>
@@ -5144,7 +5150,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>5</v>
       </c>
@@ -5165,7 +5171,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <v>6</v>
       </c>
@@ -5186,7 +5192,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <v>7</v>
       </c>
@@ -5207,7 +5213,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:18" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <v>8</v>
       </c>
@@ -5228,7 +5234,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <v>9</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <v>10</v>
       </c>
@@ -5270,7 +5276,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="20">
         <v>11</v>
       </c>
@@ -5291,7 +5297,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="20">
         <v>12</v>
       </c>
@@ -5310,7 +5316,7 @@
       </c>
       <c r="G30" s="23"/>
     </row>
-    <row r="31" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20">
         <v>13</v>
       </c>
@@ -5329,7 +5335,7 @@
       </c>
       <c r="G31" s="23"/>
     </row>
-    <row r="32" spans="2:18" s="20" customFormat="1" ht="157.69999999999999" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:18" s="20" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="B32" s="20">
         <v>14</v>
       </c>
@@ -5350,7 +5356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" s="20">
         <v>15</v>
       </c>
@@ -5371,7 +5377,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:7" s="20" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B34" s="20">
         <v>16</v>
       </c>
@@ -5392,7 +5398,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>17</v>
       </c>
@@ -5413,7 +5419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="20">
         <v>18</v>
       </c>
@@ -5434,7 +5440,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="20">
         <v>19</v>
       </c>
@@ -5455,7 +5461,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="20">
         <v>20</v>
       </c>
@@ -5476,7 +5482,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="20">
         <v>21</v>
       </c>
@@ -5495,7 +5501,7 @@
       </c>
       <c r="G39" s="23"/>
     </row>
-    <row r="40" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="20">
         <v>22</v>
       </c>
@@ -5516,7 +5522,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" s="20">
         <v>23</v>
       </c>
@@ -5537,7 +5543,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="20">
         <v>24</v>
       </c>
@@ -5558,7 +5564,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B43" s="20">
         <v>25</v>
       </c>
@@ -5579,7 +5585,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:7" s="20" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="B44" s="20">
         <v>26</v>
       </c>
@@ -5600,7 +5606,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="20">
         <v>27</v>
       </c>
@@ -5619,7 +5625,7 @@
       </c>
       <c r="G45" s="23"/>
     </row>
-    <row r="46" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="20">
         <v>28</v>
       </c>
@@ -5640,7 +5646,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:7" s="20" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="B47" s="20">
         <v>29</v>
       </c>
@@ -5661,7 +5667,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B48" s="20">
         <v>30</v>
       </c>
@@ -5680,7 +5686,7 @@
       </c>
       <c r="G48" s="23"/>
     </row>
-    <row r="49" spans="2:12" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B49" s="20">
         <v>31</v>
       </c>
@@ -5699,7 +5705,7 @@
       </c>
       <c r="G49" s="23"/>
     </row>
-    <row r="50" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" s="20">
         <v>32</v>
       </c>
@@ -5720,7 +5726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="20">
         <v>33</v>
       </c>
@@ -5739,7 +5745,7 @@
       </c>
       <c r="G51" s="23"/>
     </row>
-    <row r="52" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B52" s="20">
         <v>34</v>
       </c>
@@ -5760,7 +5766,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" s="20">
         <v>35</v>
       </c>
@@ -5779,7 +5785,7 @@
       </c>
       <c r="G53" s="23"/>
     </row>
-    <row r="54" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="20">
         <v>36</v>
       </c>
@@ -5800,7 +5806,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="20">
         <v>37</v>
       </c>
@@ -5819,7 +5825,7 @@
       </c>
       <c r="G55" s="23"/>
     </row>
-    <row r="56" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="20">
         <v>38</v>
       </c>
@@ -5835,7 +5841,7 @@
       </c>
       <c r="G56" s="23"/>
     </row>
-    <row r="57" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="B57" s="20">
         <v>39</v>
       </c>
@@ -5855,7 +5861,7 @@
       <c r="G57" s="23"/>
       <c r="L57" s="27"/>
     </row>
-    <row r="58" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="20">
         <v>40</v>
       </c>
@@ -5876,7 +5882,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="20">
         <v>41</v>
       </c>
@@ -5897,7 +5903,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B60" s="20">
         <v>42</v>
       </c>
@@ -5918,7 +5924,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="20">
         <v>43</v>
       </c>
@@ -5939,7 +5945,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="20">
         <v>44</v>
       </c>
@@ -5958,7 +5964,7 @@
       </c>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B63" s="20">
         <v>45</v>
       </c>
@@ -5977,7 +5983,7 @@
       </c>
       <c r="G63" s="23"/>
     </row>
-    <row r="64" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B64" s="20">
         <v>46</v>
       </c>
@@ -5996,7 +6002,7 @@
       </c>
       <c r="G64" s="23"/>
     </row>
-    <row r="65" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="20">
         <v>47</v>
       </c>
@@ -6015,7 +6021,7 @@
       </c>
       <c r="G65" s="23"/>
     </row>
-    <row r="66" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="20">
         <v>48</v>
       </c>
@@ -6036,7 +6042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="20">
         <v>49</v>
       </c>
@@ -6055,7 +6061,7 @@
       </c>
       <c r="G67" s="23"/>
     </row>
-    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="20">
         <v>50</v>
       </c>
@@ -6074,7 +6080,7 @@
       </c>
       <c r="G68" s="23"/>
     </row>
-    <row r="69" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="20">
         <v>51</v>
       </c>
@@ -6093,7 +6099,7 @@
       </c>
       <c r="G69" s="23"/>
     </row>
-    <row r="70" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="20">
         <v>52</v>
       </c>
@@ -6112,7 +6118,7 @@
       </c>
       <c r="G70" s="23"/>
     </row>
-    <row r="71" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="20">
         <v>53</v>
       </c>
@@ -6133,7 +6139,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:7" s="20" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="B72" s="20">
         <v>54</v>
       </c>
@@ -6154,7 +6160,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B73" s="20">
         <v>55</v>
       </c>
@@ -6175,7 +6181,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B74" s="20">
         <v>56</v>
       </c>
@@ -6196,7 +6202,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B75" s="20">
         <v>57</v>
       </c>
@@ -6217,7 +6223,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="20">
         <v>58</v>
       </c>
@@ -6238,7 +6244,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B77" s="20">
         <v>59</v>
       </c>
@@ -6259,7 +6265,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="78" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="20">
         <v>60</v>
       </c>
@@ -6280,7 +6286,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="20">
         <v>61</v>
       </c>
@@ -6301,7 +6307,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="20">
         <v>62</v>
       </c>
@@ -6320,7 +6326,7 @@
       </c>
       <c r="G80" s="23"/>
     </row>
-    <row r="81" spans="2:7" s="20" customFormat="1" ht="172" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:7" s="20" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="B81" s="20">
         <v>63</v>
       </c>
@@ -6341,7 +6347,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B82" s="20">
         <v>64</v>
       </c>
@@ -6362,7 +6368,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="20">
         <v>65</v>
       </c>
@@ -6381,7 +6387,7 @@
       </c>
       <c r="G83" s="23"/>
     </row>
-    <row r="84" spans="2:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="20">
         <v>66</v>
       </c>
@@ -6402,7 +6408,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B85" s="20">
         <v>67</v>
       </c>
@@ -6421,7 +6427,7 @@
       </c>
       <c r="G85" s="23"/>
     </row>
-    <row r="86" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B86" s="20">
         <v>68</v>
       </c>
@@ -6442,7 +6448,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B87" s="20">
         <v>69</v>
       </c>
@@ -6463,7 +6469,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="88" spans="2:7" s="20" customFormat="1" ht="229.35" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:7" s="20" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="B88" s="20">
         <v>70</v>
       </c>
@@ -6484,7 +6490,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="2:7" s="20" customFormat="1" ht="258" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:7" s="20" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="B89" s="20" t="s">
         <v>336</v>
       </c>
@@ -6505,7 +6511,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="90" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="20" t="s">
         <v>339</v>
       </c>
@@ -6526,7 +6532,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B91" s="20" t="s">
         <v>342</v>
       </c>
@@ -6545,7 +6551,7 @@
       </c>
       <c r="G91" s="58"/>
     </row>
-    <row r="92" spans="2:7" s="20" customFormat="1" ht="186.35" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:7" s="20" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="B92" s="20">
         <v>71</v>
       </c>
@@ -6566,7 +6572,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="93" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B93" s="20">
         <v>71</v>
       </c>
@@ -6587,7 +6593,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="94" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B94" s="20">
         <v>72</v>
       </c>
@@ -6608,7 +6614,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="95" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B95" s="20">
         <v>73</v>
       </c>
@@ -6627,7 +6633,7 @@
       </c>
       <c r="G95" s="23"/>
     </row>
-    <row r="96" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B96" s="20">
         <v>74</v>
       </c>
@@ -6648,7 +6654,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B97" s="20">
         <v>75</v>
       </c>
@@ -6667,7 +6673,7 @@
       </c>
       <c r="G97" s="23"/>
     </row>
-    <row r="98" spans="2:7" s="20" customFormat="1" ht="129" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:7" s="20" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="B98" s="20">
         <v>76</v>
       </c>
@@ -6688,7 +6694,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="99" spans="2:7" s="20" customFormat="1" ht="329.7" x14ac:dyDescent="0.5">
+    <row r="99" spans="2:7" s="20" customFormat="1" ht="390" x14ac:dyDescent="0.25">
       <c r="B99" s="20">
         <v>77</v>
       </c>
@@ -6709,7 +6715,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="100" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:7" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B100" s="20">
         <v>78</v>
       </c>
@@ -6730,7 +6736,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="101" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:7" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B101" s="20">
         <v>79</v>
       </c>
@@ -6751,7 +6757,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="102" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="20">
         <v>80</v>
       </c>
@@ -6772,7 +6778,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="103" spans="2:7" s="20" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B103" s="20">
         <v>81</v>
       </c>
@@ -6793,7 +6799,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="104" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="20">
         <v>82</v>
       </c>
@@ -6812,7 +6818,7 @@
       </c>
       <c r="G104" s="23"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="20">
         <v>83</v>
       </c>
@@ -6831,7 +6837,7 @@
       </c>
       <c r="G105" s="23"/>
     </row>
-    <row r="106" spans="2:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B106" s="20">
         <v>84</v>
       </c>
@@ -6852,7 +6858,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B107" s="20">
         <v>85</v>
       </c>
@@ -6871,7 +6877,7 @@
       </c>
       <c r="G107" s="23"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="20">
         <v>86</v>
       </c>
@@ -6890,7 +6896,7 @@
       </c>
       <c r="G108" s="23"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B109" s="20">
         <v>87</v>
       </c>
@@ -6911,7 +6917,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B110" s="20">
         <v>88</v>
       </c>
@@ -6930,7 +6936,7 @@
       </c>
       <c r="G110" s="23"/>
     </row>
-    <row r="111" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B111" s="20">
         <v>89</v>
       </c>
@@ -6951,7 +6957,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B112" s="20">
         <v>90</v>
       </c>
@@ -6970,7 +6976,7 @@
       </c>
       <c r="G112" s="23"/>
     </row>
-    <row r="113" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B113" s="20">
         <v>91</v>
       </c>
@@ -6989,7 +6995,7 @@
       </c>
       <c r="G113" s="23"/>
     </row>
-    <row r="114" spans="2:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="20">
         <v>92</v>
       </c>
@@ -7008,7 +7014,7 @@
       </c>
       <c r="G114" s="23"/>
     </row>
-    <row r="115" spans="2:7" ht="129" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B115" s="20">
         <v>93</v>
       </c>
@@ -7029,7 +7035,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="20">
         <v>94</v>
       </c>
@@ -7039,7 +7045,7 @@
       <c r="F116" s="23"/>
       <c r="G116" s="23"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="20">
         <v>95</v>
       </c>
@@ -7049,7 +7055,7 @@
       <c r="F117" s="23"/>
       <c r="G117" s="23"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="20">
         <v>96</v>
       </c>
@@ -7059,7 +7065,7 @@
       <c r="F118" s="23"/>
       <c r="G118" s="23"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="20">
         <v>97</v>
       </c>
@@ -7069,7 +7075,7 @@
       <c r="F119" s="23"/>
       <c r="G119" s="23"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="20">
         <v>98</v>
       </c>
@@ -7079,7 +7085,7 @@
       <c r="F120" s="23"/>
       <c r="G120" s="23"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="20">
         <v>99</v>
       </c>
@@ -7089,7 +7095,7 @@
       <c r="F121" s="23"/>
       <c r="G121" s="23"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="20">
         <v>100</v>
       </c>
@@ -7124,21 +7130,21 @@
       <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="2" width="92.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1171875" customWidth="1"/>
-    <col min="4" max="5" width="16.703125" customWidth="1"/>
-    <col min="6" max="17" width="16.703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="17" width="16.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="70" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" s="70" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="70" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -7158,7 +7164,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -7177,7 +7183,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -7196,7 +7202,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -7209,12 +7215,12 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:17" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="71" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -7227,7 +7233,7 @@
       <c r="P9"/>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>187</v>
       </c>
@@ -7249,7 +7255,7 @@
       <c r="P10" s="72"/>
       <c r="Q10" s="72"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>190</v>
       </c>
@@ -7263,7 +7269,7 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>192</v>
       </c>
@@ -7277,7 +7283,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>191</v>
       </c>
@@ -7291,80 +7297,80 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="15" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:17" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="71" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="16" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f t="shared" ref="B37:B43" si="0">D38</f>
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
@@ -7383,7 +7389,7 @@
       <c r="P37"/>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>Gas Control Device/Control System Component</v>
@@ -7402,7 +7408,7 @@
       <c r="P38"/>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Daily Cover</v>
@@ -7420,7 +7426,7 @@
       <c r="P39"/>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Final Cover</v>
@@ -7438,7 +7444,7 @@
       <c r="P40"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Intermediate Cover</v>
@@ -7456,7 +7462,7 @@
       <c r="P41"/>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>Leachate Management System</v>
@@ -7474,7 +7480,7 @@
       <c r="P42"/>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
@@ -7492,25 +7498,25 @@
       <c r="P43"/>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D44" s="7" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="16"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="66" t="str" cm="1">
         <f t="array" ref="B48:B58">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.TOCOL(C64:M70, 1)))</f>
         <v>Collection system downtime</v>
@@ -7518,89 +7524,89 @@
       <c r="E48" s="7"/>
       <c r="Q48"/>
     </row>
-    <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="68" t="str">
         <v>Construction - New Well Installation</v>
       </c>
       <c r="E49" s="7"/>
       <c r="Q49"/>
     </row>
-    <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="69" t="str">
         <v>Construction - Well Raising or Horizontal Extension</v>
       </c>
       <c r="E50" s="7"/>
       <c r="Q50"/>
     </row>
-    <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="67" t="str">
         <v>Cover integrity</v>
       </c>
       <c r="E51" s="7"/>
       <c r="Q51"/>
     </row>
-    <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="66" t="str">
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
       <c r="E52" s="7"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="67" t="str">
         <v>Cracked/Broken Seal</v>
       </c>
       <c r="E53" s="7"/>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="66" t="str">
         <v>Damaged component</v>
       </c>
       <c r="E54" s="7"/>
       <c r="Q54"/>
     </row>
-    <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="66" t="str">
         <v>Insufficient vacuum</v>
       </c>
       <c r="E55" s="7"/>
       <c r="Q55"/>
     </row>
-    <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="68" t="str">
         <v>Offline Gas Collection Well(s)</v>
       </c>
       <c r="E56" s="7"/>
       <c r="Q56"/>
     </row>
-    <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="69" t="str">
         <v>Other</v>
       </c>
       <c r="E57" s="7"/>
       <c r="Q57"/>
     </row>
-    <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="67" t="str">
         <v>Uncontrolled Area (no gas collection infrastructure)</v>
       </c>
       <c r="E58" s="7"/>
       <c r="Q58"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="2:17" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="62" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>176</v>
       </c>
@@ -7608,7 +7614,7 @@
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="2:17" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>177</v>
       </c>
@@ -7618,7 +7624,7 @@
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="2:17" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:17" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
         <v>399</v>
       </c>
@@ -7646,7 +7652,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
         <v>167</v>
       </c>
@@ -7684,7 +7690,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
         <v>168</v>
       </c>
@@ -7722,7 +7728,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="67" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>169</v>
       </c>
@@ -7758,7 +7764,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
         <v>170</v>
       </c>
@@ -7782,7 +7788,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>186</v>
       </c>
@@ -7812,7 +7818,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
         <v>13</v>
       </c>
@@ -7834,12 +7840,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" t="str" cm="1">
         <f t="array" ref="B74:C125">_xlfn.HSTACK(_xlfn.TOCOL(_xlfn.IFS(C64:M70&lt;&gt;"",B64:B70),3),_xlfn.TOCOL(C64:M70,1))</f>
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
@@ -7849,7 +7855,7 @@
       </c>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7858,7 +7864,7 @@
       </c>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7867,7 +7873,7 @@
       </c>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B77" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7876,7 +7882,7 @@
       </c>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7885,7 +7891,7 @@
       </c>
       <c r="G78"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7894,7 +7900,7 @@
       </c>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B80" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7903,7 +7909,7 @@
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7912,7 +7918,7 @@
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7921,7 +7927,7 @@
       </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7930,7 +7936,7 @@
       </c>
       <c r="G83"/>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7939,7 +7945,7 @@
       </c>
       <c r="G84"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7948,7 +7954,7 @@
       </c>
       <c r="G85"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7957,7 +7963,7 @@
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7966,7 +7972,7 @@
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7975,7 +7981,7 @@
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7984,7 +7990,7 @@
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7993,7 +7999,7 @@
       </c>
       <c r="G90"/>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8002,7 +8008,7 @@
       </c>
       <c r="G91"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8011,7 +8017,7 @@
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8020,7 +8026,7 @@
       </c>
       <c r="G93"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8029,7 +8035,7 @@
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8038,7 +8044,7 @@
       </c>
       <c r="G95"/>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8047,7 +8053,7 @@
       </c>
       <c r="G96"/>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8056,7 +8062,7 @@
       </c>
       <c r="G97"/>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8065,7 +8071,7 @@
       </c>
       <c r="G98"/>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8074,7 +8080,7 @@
       </c>
       <c r="G99"/>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8083,7 +8089,7 @@
       </c>
       <c r="G100"/>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8092,7 +8098,7 @@
       </c>
       <c r="G101"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8101,7 +8107,7 @@
       </c>
       <c r="G102"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8110,7 +8116,7 @@
       </c>
       <c r="G103"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8119,7 +8125,7 @@
       </c>
       <c r="G104"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8128,7 +8134,7 @@
       </c>
       <c r="G105"/>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8137,7 +8143,7 @@
       </c>
       <c r="G106"/>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8146,7 +8152,7 @@
       </c>
       <c r="G107"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8155,7 +8161,7 @@
       </c>
       <c r="G108"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8164,7 +8170,7 @@
       </c>
       <c r="G109"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8173,7 +8179,7 @@
       </c>
       <c r="G110"/>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8182,7 +8188,7 @@
       </c>
       <c r="G111"/>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8191,7 +8197,7 @@
       </c>
       <c r="G112"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8200,7 +8206,7 @@
       </c>
       <c r="G113"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8209,7 +8215,7 @@
       </c>
       <c r="G114"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8218,7 +8224,7 @@
       </c>
       <c r="G115"/>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8227,7 +8233,7 @@
       </c>
       <c r="G116"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8236,7 +8242,7 @@
       </c>
       <c r="G117"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8245,7 +8251,7 @@
       </c>
       <c r="G118"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8254,7 +8260,7 @@
       </c>
       <c r="G119"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8263,7 +8269,7 @@
       </c>
       <c r="G120"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8272,7 +8278,7 @@
       </c>
       <c r="G121"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8281,7 +8287,7 @@
       </c>
       <c r="G122"/>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8289,7 +8295,7 @@
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8298,7 +8304,7 @@
       </c>
       <c r="G124"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8307,21 +8313,21 @@
       </c>
       <c r="G125"/>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G126"/>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G134"/>
     </row>
-    <row r="135" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="135" spans="2:7" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B135" s="71" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G136"/>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="17" t="s">
         <v>193</v>
       </c>
@@ -8330,12 +8336,12 @@
       </c>
       <c r="G137"/>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="16"/>
       <c r="C138" s="16"/>
       <c r="G138"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>163</v>
       </c>
@@ -8345,7 +8351,7 @@
       </c>
       <c r="G139"/>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" t="str" cm="1">
         <f t="array" ref="B140:B142">_carb_only_table_02[]</f>
         <v>Operator was aware of the leak prior to receiving the CARB plume notification</v>
@@ -8355,7 +8361,7 @@
       </c>
       <c r="G140"/>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" t="str">
         <v>Operator detected a leak during follow-up monitoring after receipt of the CARB plume notification</v>
       </c>
@@ -8364,7 +8370,7 @@
       </c>
       <c r="G141"/>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" t="str">
         <v>No leak was detected</v>
       </c>
@@ -8373,18 +8379,18 @@
       </c>
       <c r="G142"/>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G143"/>
     </row>
-    <row r="144" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="144" spans="2:7" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B144" s="71" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G145"/>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="17" t="s">
         <v>193</v>
       </c>
@@ -8393,12 +8399,12 @@
       </c>
       <c r="G146"/>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="16"/>
       <c r="C147" s="16"/>
       <c r="G147"/>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>163</v>
       </c>
@@ -8408,7 +8414,7 @@
       </c>
       <c r="G148"/>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8419,7 +8425,7 @@
       </c>
       <c r="G149"/>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" t="str" cm="1">
         <f t="array" ref="B150:B153">_carb_only_table_03[]</f>
         <v>Operator was aware of the leak prior to receiving the notification, and/or repairs were in progress on the date of the plume observation</v>
@@ -8430,7 +8436,7 @@
       </c>
       <c r="G150"/>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" t="str">
         <v>An unintentional leak  (i.e., the operator was not aware of, and could be repaired if discovered)</v>
       </c>
@@ -8440,7 +8446,7 @@
       </c>
       <c r="G151"/>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" t="str">
         <v>An intentional or allowable vent (i.e., the operator was aware of, and/or would not repair)</v>
       </c>
@@ -8450,24 +8456,24 @@
       </c>
       <c r="G152"/>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" t="str">
         <v>Due to a temporary activity (i.e., would be resolved without corrective action when the activity is complete)</v>
       </c>
       <c r="G153"/>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G154"/>
     </row>
-    <row r="155" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="155" spans="2:7" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B155" s="71" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G156"/>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="17" t="s">
         <v>193</v>
       </c>
@@ -8476,12 +8482,12 @@
       </c>
       <c r="G157"/>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="16"/>
       <c r="C158" s="16"/>
       <c r="G158"/>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>163</v>
       </c>
@@ -8491,7 +8497,7 @@
       </c>
       <c r="G159"/>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8502,7 +8508,7 @@
       </c>
       <c r="G160"/>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161" t="str" cm="1">
         <f t="array" ref="B161:B167">_carb_only_table_04[]</f>
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
@@ -8513,7 +8519,7 @@
       </c>
       <c r="G161"/>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8523,7 +8529,7 @@
       </c>
       <c r="G162"/>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -8533,7 +8539,7 @@
       </c>
       <c r="G163"/>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8543,7 +8549,7 @@
       </c>
       <c r="G164"/>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8553,7 +8559,7 @@
       </c>
       <c r="G165"/>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8563,24 +8569,24 @@
       </c>
       <c r="G166"/>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
       <c r="G167"/>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G168"/>
     </row>
-    <row r="169" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="169" spans="2:7" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B169" s="71" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G170"/>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B171" s="17" t="s">
         <v>193</v>
       </c>
@@ -8589,12 +8595,12 @@
       </c>
       <c r="G171"/>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="16"/>
       <c r="C172" s="16"/>
       <c r="G172"/>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>163</v>
       </c>
@@ -8604,7 +8610,7 @@
       </c>
       <c r="G173"/>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B174" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8615,7 +8621,7 @@
       </c>
       <c r="G174"/>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175" t="str" cm="1">
         <f t="array" aca="1" ref="B175:B181" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
         <v>Offline Gas Collection Well(s)</v>
@@ -8626,7 +8632,7 @@
       </c>
       <c r="G175"/>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B176" t="str">
         <f ca="1"/>
         <v>Construction - New Well Installation</v>
@@ -8637,7 +8643,7 @@
       </c>
       <c r="G176"/>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B177" t="str">
         <f ca="1"/>
         <v>Construction - Well Raising or Horizontal Extension</v>
@@ -8648,7 +8654,7 @@
       </c>
       <c r="G177"/>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B178" t="str">
         <f ca="1"/>
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
@@ -8659,7 +8665,7 @@
       </c>
       <c r="G178"/>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179" t="str">
         <f ca="1"/>
         <v>Damaged component</v>
@@ -8670,7 +8676,7 @@
       </c>
       <c r="G179"/>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180" t="str">
         <f ca="1"/>
         <v>Insufficient vacuum</v>
@@ -8681,49 +8687,49 @@
       </c>
       <c r="G180"/>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" t="str">
         <f ca="1"/>
         <v>Other</v>
       </c>
       <c r="G181"/>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G182"/>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G183"/>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G184"/>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G185"/>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G186"/>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G187"/>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G188"/>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G189"/>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G190"/>
     </row>
-    <row r="191" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="191" spans="2:7" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B191" s="71" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G192"/>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="17" t="s">
         <v>193</v>
       </c>
@@ -8732,12 +8738,12 @@
       </c>
       <c r="G193"/>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="16"/>
       <c r="C194" s="16"/>
       <c r="G194"/>
     </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>163</v>
       </c>
@@ -8747,7 +8753,7 @@
       </c>
       <c r="G195"/>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8758,7 +8764,7 @@
       </c>
       <c r="G196"/>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>355</v>
       </c>
@@ -8768,7 +8774,7 @@
       </c>
       <c r="G197"/>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B198" t="str" cm="1">
         <f t="array" aca="1" ref="B198:B204" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
         <v>Offline Gas Collection Well(s)</v>
@@ -8779,7 +8785,7 @@
       </c>
       <c r="G198"/>
     </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B199" t="str">
         <f ca="1"/>
         <v>Construction - New Well Installation</v>
@@ -8790,7 +8796,7 @@
       </c>
       <c r="G199"/>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B200" t="str">
         <f ca="1"/>
         <v>Construction - Well Raising or Horizontal Extension</v>
@@ -8801,7 +8807,7 @@
       </c>
       <c r="G200"/>
     </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B201" t="str">
         <f ca="1"/>
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
@@ -8812,7 +8818,7 @@
       </c>
       <c r="G201"/>
     </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" t="str">
         <f ca="1"/>
         <v>Damaged component</v>
@@ -8823,7 +8829,7 @@
       </c>
       <c r="G202"/>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" t="str">
         <f ca="1"/>
         <v>Insufficient vacuum</v>
@@ -8834,41 +8840,41 @@
       </c>
       <c r="G203"/>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B204" t="str">
         <f ca="1"/>
         <v>Other</v>
       </c>
       <c r="G204"/>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G205"/>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G206"/>
     </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G207"/>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G208"/>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G209"/>
     </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G210"/>
     </row>
-    <row r="213" spans="2:7" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="213" spans="2:7" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B213" s="71" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B214" s="16"/>
       <c r="G214"/>
     </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B215" s="17" t="s">
         <v>193</v>
       </c>
@@ -8877,12 +8883,12 @@
       </c>
       <c r="G215"/>
     </row>
-    <row r="216" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B216" s="16"/>
       <c r="C216" s="16"/>
       <c r="G216"/>
     </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>163</v>
       </c>
@@ -8892,7 +8898,7 @@
       </c>
       <c r="G217"/>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B218" t="str" cm="1">
         <f t="array" ref="B218:B219">_carb_only_table_01[]</f>
         <v>Yes</v>
@@ -8902,7 +8908,7 @@
       </c>
       <c r="G218"/>
     </row>
-    <row r="219" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" t="str">
         <v>No</v>
       </c>
@@ -8931,19 +8937,19 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="30.703125" customWidth="1"/>
-    <col min="4" max="9" width="8.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8951,7 +8957,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8959,7 +8965,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8967,7 +8973,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -8975,7 +8981,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
         <v>200</v>
       </c>
@@ -8983,7 +8989,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>202</v>
       </c>
@@ -9006,18 +9012,18 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="30.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -9025,7 +9031,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -9033,7 +9039,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -9041,7 +9047,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -9049,12 +9055,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
         <v>206</v>
       </c>
@@ -9062,7 +9068,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>208</v>
       </c>
@@ -9070,7 +9076,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>210</v>
       </c>
@@ -9094,24 +9100,24 @@
       <selection activeCell="A11" sqref="A11:F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="2" width="25.1171875" customWidth="1"/>
-    <col min="3" max="3" width="16.41015625" customWidth="1"/>
-    <col min="4" max="4" width="32.41015625" customWidth="1"/>
-    <col min="5" max="5" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>212</v>
       </c>
       <c r="C2" s="22"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -9121,26 +9127,26 @@
       <c r="C4" s="1"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:6" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:6" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>200</v>
       </c>
@@ -9157,7 +9163,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>350</v>
       </c>
@@ -9174,7 +9180,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>350</v>
       </c>
@@ -9191,7 +9197,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>202</v>
       </c>
@@ -9208,7 +9214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>202</v>
       </c>
@@ -9225,7 +9231,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>202</v>
       </c>
@@ -9242,7 +9248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>202</v>
       </c>
@@ -9259,7 +9265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>202</v>
       </c>
@@ -9276,7 +9282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>202</v>
       </c>
@@ -9293,7 +9299,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>202</v>
       </c>
@@ -9310,7 +9316,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>202</v>
       </c>
@@ -9327,7 +9333,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>202</v>
       </c>
@@ -9344,7 +9350,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>202</v>
       </c>
@@ -9361,7 +9367,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>202</v>
       </c>
@@ -9378,7 +9384,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>202</v>
       </c>
@@ -9395,7 +9401,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>202</v>
       </c>
@@ -9412,7 +9418,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>202</v>
       </c>
@@ -9429,7 +9435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>202</v>
       </c>
@@ -9446,7 +9452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>202</v>
       </c>
@@ -9463,7 +9469,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>202</v>
       </c>
@@ -9480,7 +9486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>202</v>
       </c>
@@ -9497,7 +9503,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>202</v>
       </c>
@@ -9514,7 +9520,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>202</v>
       </c>
@@ -9531,7 +9537,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>202</v>
       </c>
@@ -9548,7 +9554,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>202</v>
       </c>
@@ -9565,7 +9571,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>202</v>
       </c>
@@ -9582,7 +9588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>202</v>
       </c>
@@ -9599,7 +9605,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>202</v>
       </c>
@@ -9616,7 +9622,7 @@
         <v>45276</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>202</v>
       </c>
@@ -9633,7 +9639,7 @@
         <v>35.321100000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>202</v>
       </c>
@@ -9650,7 +9656,7 @@
         <v>35.321100000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>202</v>
       </c>
@@ -9667,7 +9673,7 @@
         <v>-119.5808</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>202</v>
       </c>
@@ -9684,7 +9690,7 @@
         <v>-119.5808</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>202</v>
       </c>
@@ -9701,7 +9707,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>202</v>
       </c>
@@ -9718,7 +9724,7 @@
         <v>45275</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>202</v>
       </c>
@@ -9735,7 +9741,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>202</v>
       </c>
@@ -9752,7 +9758,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>202</v>
       </c>
@@ -9769,7 +9775,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>202</v>
       </c>
@@ -9786,7 +9792,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>202</v>
       </c>
@@ -9823,29 +9829,29 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.87890625" customWidth="1"/>
-    <col min="5" max="5" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.29296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.29296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.29296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:13" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>418</v>
       </c>
       <c r="C2" s="22"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="6" spans="2:13" ht="86" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:13" ht="90" x14ac:dyDescent="0.25">
       <c r="B6" s="77" t="s">
         <v>406</v>
       </c>
@@ -9883,7 +9889,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="79"/>
       <c r="C7" s="79"/>
       <c r="D7" s="79"/>
@@ -9897,7 +9903,7 @@
       <c r="L7" s="79"/>
       <c r="M7" s="79"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="79"/>
       <c r="C8" s="79"/>
       <c r="D8" s="79"/>
@@ -9911,7 +9917,7 @@
       <c r="L8" s="79"/>
       <c r="M8" s="79"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="79"/>
       <c r="C9" s="79"/>
       <c r="D9" s="79"/>
@@ -9925,7 +9931,7 @@
       <c r="L9" s="79"/>
       <c r="M9" s="79"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="79"/>
       <c r="C10" s="79"/>
       <c r="D10" s="79"/>
@@ -9939,7 +9945,7 @@
       <c r="L10" s="79"/>
       <c r="M10" s="79"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="79"/>
       <c r="C11" s="79"/>
       <c r="D11" s="79"/>
@@ -9953,7 +9959,7 @@
       <c r="L11" s="79"/>
       <c r="M11" s="79"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
       <c r="D12" s="79"/>
@@ -9967,7 +9973,7 @@
       <c r="L12" s="79"/>
       <c r="M12" s="79"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="79"/>
       <c r="C13" s="79"/>
       <c r="D13" s="79"/>
@@ -9981,7 +9987,7 @@
       <c r="L13" s="79"/>
       <c r="M13" s="79"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="79"/>
       <c r="C14" s="79"/>
       <c r="D14" s="79"/>
@@ -9995,7 +10001,7 @@
       <c r="L14" s="79"/>
       <c r="M14" s="79"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
       <c r="D15" s="79"/>
@@ -10009,7 +10015,7 @@
       <c r="L15" s="79"/>
       <c r="M15" s="79"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="79"/>
       <c r="C16" s="79"/>
       <c r="D16" s="79"/>
@@ -10023,7 +10029,7 @@
       <c r="L16" s="79"/>
       <c r="M16" s="79"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="79"/>
       <c r="C17" s="79"/>
       <c r="D17" s="79"/>
@@ -10037,7 +10043,7 @@
       <c r="L17" s="79"/>
       <c r="M17" s="79"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="79"/>
       <c r="C18" s="79"/>
       <c r="D18" s="79"/>
@@ -10051,7 +10057,7 @@
       <c r="L18" s="79"/>
       <c r="M18" s="79"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="79"/>
       <c r="C19" s="79"/>
       <c r="D19" s="79"/>
@@ -10065,7 +10071,7 @@
       <c r="L19" s="79"/>
       <c r="M19" s="79"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="79"/>
       <c r="C20" s="79"/>
       <c r="D20" s="79"/>
@@ -10079,7 +10085,7 @@
       <c r="L20" s="79"/>
       <c r="M20" s="79"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="79"/>
       <c r="C21" s="79"/>
       <c r="D21" s="79"/>
@@ -10093,7 +10099,7 @@
       <c r="L21" s="79"/>
       <c r="M21" s="79"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="79"/>
       <c r="C22" s="79"/>
       <c r="D22" s="79"/>
@@ -10107,7 +10113,7 @@
       <c r="L22" s="79"/>
       <c r="M22" s="79"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="79"/>
       <c r="C23" s="79"/>
       <c r="D23" s="79"/>
@@ -10121,7 +10127,7 @@
       <c r="L23" s="79"/>
       <c r="M23" s="79"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="79"/>
       <c r="C24" s="79"/>
       <c r="D24" s="79"/>
@@ -10135,7 +10141,7 @@
       <c r="L24" s="79"/>
       <c r="M24" s="79"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="79"/>
       <c r="C25" s="79"/>
       <c r="D25" s="79"/>
@@ -10149,7 +10155,7 @@
       <c r="L25" s="79"/>
       <c r="M25" s="79"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="79"/>
       <c r="C26" s="79"/>
       <c r="D26" s="79"/>
@@ -10170,12 +10176,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10414,20 +10422,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10452,12 +10461,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>